<commit_message>
Se agregaron mas requerimientos
</commit_message>
<xml_diff>
--- a/TRIMESTRE I/04_REQUISITOS FUNCIONALES Y NO FUNCIONALES/Requerimientos.xlsx
+++ b/TRIMESTRE I/04_REQUISITOS FUNCIONALES Y NO FUNCIONALES/Requerimientos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af6a0e1bbe79e0f6/Escritorio/proyect/SENA/TRIMESTRE I/04_REQUISITOS FUNCIONALES Y NO FUNCIONALES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\SENA\TRIMESTRE I\04_REQUISITOS FUNCIONALES Y NO FUNCIONALES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{E685D32E-949E-4989-BECC-27639FAD37A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{779028B3-BE32-4B1A-8915-0D98E7656139}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29431B9F-C2B6-4189-AB77-3B237EA9C4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipo" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
   <si>
     <t>#</t>
   </si>
@@ -290,13 +290,46 @@
   </si>
   <si>
     <t>La plataforma debe ser compatible con los navegadores más utilizados (Chrome, Firefox, Safari, Edge), La página debe ser funcional en dispositivos móviles, tablets y ordenadores de escritorio, garantizando una experiencia óptima en cada dispositivo.</t>
+  </si>
+  <si>
+    <t>Recuperar contraseña</t>
+  </si>
+  <si>
+    <t>Pagos</t>
+  </si>
+  <si>
+    <t>Permitir al usuario recuperar su contraseña</t>
+  </si>
+  <si>
+    <t>RE_</t>
+  </si>
+  <si>
+    <t>El sistema le ofrecera diferentes medios de pago para realizar la compra</t>
+  </si>
+  <si>
+    <t>RE_014</t>
+  </si>
+  <si>
+    <t>Base de datos</t>
+  </si>
+  <si>
+    <t>El sistema contará con una base de datos para almacenar datos como nombres o contraseñas, adicional, el usuario con el rol de administrador será capaz de acceder a la base de datos para buscar, editar, eliminar, crear, modificar datos dentro de la base de dato</t>
+  </si>
+  <si>
+    <t>RE_015</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>El sistema debe enviar notificaciones y confirmaciones por correo electrónico o mensajes de texto para informar a los usuarios sobre el estado de sus compras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,6 +370,19 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -352,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -377,12 +423,29 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -391,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -408,8 +471,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1798,10 +1870,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:G1002"/>
+  <dimension ref="B1:G1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1815,301 +1887,388 @@
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="7">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="7">
         <v>2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="7">
         <v>3</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="2:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="7">
+        <v>5</v>
+      </c>
+      <c r="G12" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F14" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G14" s="7">
         <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="57" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="57" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="2">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="57" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
+      <c r="G15" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="7">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D18" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F18" s="7">
         <v>3</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G18" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+    <row r="19" spans="2:7" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F19" s="7">
         <v>2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G19" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:7" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="7">
+        <v>5</v>
+      </c>
+      <c r="G20" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="7">
+        <v>5</v>
+      </c>
+      <c r="G21" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3080,16 +3239,19 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F16 G14:G16" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F21 G17:G21" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C13" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C16" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Funcional,No Funcional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G13" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G16" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Historias de usuario actualizadas
</commit_message>
<xml_diff>
--- a/TRIMESTRE I/04_REQUISITOS FUNCIONALES Y NO FUNCIONALES/Requerimientos.xlsx
+++ b/TRIMESTRE I/04_REQUISITOS FUNCIONALES Y NO FUNCIONALES/Requerimientos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\SENA\TRIMESTRE I\04_REQUISITOS FUNCIONALES Y NO FUNCIONALES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af6a0e1bbe79e0f6/Escritorio/fede/SENA/TRIMESTRE I/04_REQUISITOS FUNCIONALES Y NO FUNCIONALES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29431B9F-C2B6-4189-AB77-3B237EA9C4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{29431B9F-C2B6-4189-AB77-3B237EA9C4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39810E04-CCEA-4D04-8A0A-8D0F6CCDE541}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipo" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>#</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Permitir al usuario recuperar su contraseña</t>
   </si>
   <si>
-    <t>RE_</t>
-  </si>
-  <si>
     <t>El sistema le ofrecera diferentes medios de pago para realizar la compra</t>
   </si>
   <si>
@@ -323,6 +320,15 @@
   </si>
   <si>
     <t>El sistema debe enviar notificaciones y confirmaciones por correo electrónico o mensajes de texto para informar a los usuarios sobre el estado de sus compras</t>
+  </si>
+  <si>
+    <t>RE_016</t>
+  </si>
+  <si>
+    <t>RE_017</t>
+  </si>
+  <si>
+    <t>RE_018</t>
   </si>
 </sst>
 </file>
@@ -1873,12 +1879,12 @@
   <dimension ref="B1:G1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="52.7109375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
@@ -2048,7 +2054,7 @@
     </row>
     <row r="11" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>13</v>
@@ -2060,7 +2066,7 @@
     </row>
     <row r="12" spans="2:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
@@ -2069,7 +2075,7 @@
         <v>88</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="7">
         <v>5</v>
@@ -2080,7 +2086,7 @@
     </row>
     <row r="13" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>13</v>
@@ -2100,7 +2106,7 @@
     </row>
     <row r="14" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>43</v>
@@ -2120,7 +2126,7 @@
     </row>
     <row r="15" spans="2:7" ht="57" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>43</v>
@@ -2140,7 +2146,7 @@
     </row>
     <row r="16" spans="2:7" ht="85.5" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>43</v>
@@ -2160,7 +2166,7 @@
     </row>
     <row r="17" spans="2:7" ht="57" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>43</v>
@@ -2180,7 +2186,7 @@
     </row>
     <row r="18" spans="2:7" ht="57" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>43</v>
@@ -2200,7 +2206,7 @@
     </row>
     <row r="19" spans="2:7" ht="142.5" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>43</v>
@@ -2220,16 +2226,16 @@
     </row>
     <row r="20" spans="2:7" ht="156.75" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="F20" s="7">
         <v>5</v>
@@ -2240,16 +2246,16 @@
     </row>
     <row r="21" spans="2:7" ht="99.75" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="F21" s="7">
         <v>5</v>

</xml_diff>